<commit_message>
Adapt to Extends columns on Excel sheets.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiPostSample.xlsx
+++ b/meta/api/BlancoApiPostSample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="460" windowWidth="21420" windowHeight="14880" tabRatio="860"/>
+    <workbookView xWindow="2560" yWindow="460" windowWidth="21420" windowHeight="14880" tabRatio="860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="200">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2101,6 +2101,56 @@
   </si>
   <si>
     <t>BlancoApiPostSampleDeleteResponse</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>電文処理定義・継承</t>
+    <rPh sb="0" eb="2">
+      <t>デンブn</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ショリ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>クラス名</t>
+  </si>
+  <si>
+    <t>パッケージ</t>
+  </si>
+  <si>
+    <t>名前空間</t>
+    <rPh sb="0" eb="4">
+      <t>ナマエクウカｎ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ApiBase</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>電文定義・継承</t>
+    <rPh sb="0" eb="2">
+      <t>デンブn</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>blanco.rest.common</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>blanco\rest\common</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>blanco.rest.valueobject</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>blanco\rest\valueobject</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -2172,7 +2222,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2209,8 +2259,32 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+        <bgColor indexed="27"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+        <bgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -2573,6 +2647,186 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2581,7 +2835,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2735,7 +2989,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2773,8 +3026,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2787,6 +3038,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2794,30 +3051,54 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -3359,10 +3640,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3447,7 +3728,7 @@
       <c r="C9" s="29"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="105" t="s">
+      <c r="A10" s="104" t="s">
         <v>167</v>
       </c>
       <c r="B10" s="58" t="s">
@@ -3456,16 +3737,16 @@
       <c r="C10" s="29"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="105" t="s">
+      <c r="A11" s="104" t="s">
         <v>168</v>
       </c>
-      <c r="B11" s="109" t="s">
+      <c r="B11" s="106" t="s">
         <v>185</v>
       </c>
       <c r="C11" s="29"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="105" t="s">
+      <c r="A12" s="104" t="s">
         <v>169</v>
       </c>
       <c r="B12" s="58" t="s">
@@ -3474,7 +3755,7 @@
       <c r="C12" s="29"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="105" t="s">
+      <c r="A13" s="104" t="s">
         <v>170</v>
       </c>
       <c r="B13" s="58" t="s">
@@ -3483,7 +3764,7 @@
       <c r="C13" s="29"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="105" t="s">
+      <c r="A14" s="104" t="s">
         <v>171</v>
       </c>
       <c r="B14" s="58" t="s">
@@ -3492,7 +3773,7 @@
       <c r="C14" s="29"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="105" t="s">
+      <c r="A15" s="104" t="s">
         <v>172</v>
       </c>
       <c r="B15" s="58" t="s">
@@ -3501,13 +3782,13 @@
       <c r="C15" s="29"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="105" t="s">
+      <c r="A16" s="104" t="s">
         <v>143</v>
       </c>
-      <c r="B16" s="106"/>
+      <c r="B16" s="105"/>
       <c r="C16" s="29"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
@@ -3516,7 +3797,7 @@
       </c>
       <c r="C17" s="29"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
@@ -3524,7 +3805,7 @@
       <c r="C18" s="61"/>
       <c r="D18" s="61"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>106</v>
       </c>
@@ -3534,7 +3815,7 @@
       <c r="C19" s="61"/>
       <c r="D19" s="61"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
@@ -3544,88 +3825,113 @@
       <c r="C20" s="61"/>
       <c r="D20" s="61"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="4" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A21" s="61"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+    </row>
+    <row r="22" spans="1:10" s="123" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="121" t="s">
+        <v>190</v>
+      </c>
+      <c r="B22" s="122"/>
+      <c r="C22" s="122"/>
+      <c r="D22" s="122"/>
+      <c r="E22" s="122"/>
+      <c r="F22" s="133"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" s="123" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="124" t="s">
+        <v>191</v>
+      </c>
+      <c r="B23" s="125"/>
+      <c r="C23" s="126" t="s">
+        <v>194</v>
+      </c>
+      <c r="D23" s="126"/>
+      <c r="E23" s="126"/>
+      <c r="F23" s="134"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" s="123" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="127" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" s="128"/>
+      <c r="C24" s="129" t="s">
+        <v>196</v>
+      </c>
+      <c r="D24" s="130"/>
+      <c r="E24" s="131"/>
+      <c r="F24" s="132"/>
+    </row>
+    <row r="25" spans="1:10" s="123" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="127" t="s">
+        <v>193</v>
+      </c>
+      <c r="B25" s="128"/>
+      <c r="C25" s="135" t="s">
+        <v>197</v>
+      </c>
+      <c r="D25" s="136"/>
+      <c r="E25" s="137"/>
+      <c r="F25" s="132"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A27" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="31" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A28" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="110" t="s">
+      <c r="B28" s="107" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="111"/>
-      <c r="D23" s="112"/>
-      <c r="E23" s="31" t="s">
+      <c r="C28" s="108"/>
+      <c r="D28" s="109"/>
+      <c r="E28" s="31" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="52"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="52"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="52"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="52"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="52"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="52"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="52"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="52"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="52"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="52"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A29" s="52"/>
       <c r="B29" s="3"/>
       <c r="C29" s="29"/>
       <c r="D29" s="54"/>
       <c r="E29" s="52"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A30" s="52"/>
       <c r="B30" s="3"/>
       <c r="C30" s="29"/>
       <c r="D30" s="54"/>
       <c r="E30" s="52"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A31" s="52"/>
       <c r="B31" s="3"/>
       <c r="C31" s="29"/>
       <c r="D31" s="54"/>
       <c r="E31" s="52"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A32" s="52"/>
       <c r="B32" s="3"/>
       <c r="C32" s="29"/>
@@ -3738,15 +4044,50 @@
       <c r="E47" s="52"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="53"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="56"/>
-      <c r="E48" s="53"/>
+      <c r="A48" s="52"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="52"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A49" s="52"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="54"/>
+      <c r="E49" s="52"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A50" s="52"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="52"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A51" s="52"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="54"/>
+      <c r="E51" s="52"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A52" s="52"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="54"/>
+      <c r="E52" s="52"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A53" s="53"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="55"/>
+      <c r="D53" s="56"/>
+      <c r="E53" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B28:D28"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.11811023622047245"/>
@@ -3774,10 +4115,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R48"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3834,7 +4175,7 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="107"/>
+      <c r="E5" s="61"/>
       <c r="F5" s="29"/>
       <c r="G5" s="29"/>
     </row>
@@ -3847,7 +4188,7 @@
         <v>182</v>
       </c>
       <c r="D6" s="37"/>
-      <c r="E6" s="108"/>
+      <c r="E6" s="61"/>
       <c r="F6" s="29"/>
       <c r="G6" s="29"/>
     </row>
@@ -3860,7 +4201,7 @@
         <v>179</v>
       </c>
       <c r="D7" s="37"/>
-      <c r="E7" s="108"/>
+      <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
       <c r="H7" s="61"/>
@@ -3876,8 +4217,8 @@
       <c r="C8" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="91"/>
-      <c r="E8" s="29"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="61"/>
       <c r="F8" s="29"/>
       <c r="G8" s="29"/>
     </row>
@@ -3886,11 +4227,11 @@
         <v>155</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="90" t="s">
+      <c r="C9" s="139" t="s">
         <v>164</v>
       </c>
-      <c r="D9" s="104"/>
-      <c r="E9" s="29"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="61"/>
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
     </row>
@@ -3901,7 +4242,7 @@
       <c r="B10" s="5"/>
       <c r="C10" s="59"/>
       <c r="D10" s="37"/>
-      <c r="E10" s="108"/>
+      <c r="E10" s="61"/>
       <c r="G10" s="29"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
@@ -3939,8 +4280,8 @@
         <v>160</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="90"/>
-      <c r="D14" s="104"/>
+      <c r="C14" s="139"/>
+      <c r="D14" s="103"/>
       <c r="E14" s="61"/>
       <c r="G14" s="29"/>
     </row>
@@ -3949,8 +4290,8 @@
         <v>161</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="90"/>
-      <c r="D15" s="104"/>
+      <c r="C15" s="139"/>
+      <c r="D15" s="103"/>
       <c r="E15" s="61"/>
       <c r="G15" s="29"/>
     </row>
@@ -3959,8 +4300,8 @@
         <v>162</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="90"/>
-      <c r="D16" s="104"/>
+      <c r="C16" s="139"/>
+      <c r="D16" s="103"/>
       <c r="E16" s="61"/>
       <c r="G16" s="29"/>
     </row>
@@ -4002,234 +4343,221 @@
       <c r="A20" s="6"/>
       <c r="C20" s="29"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A21" s="6"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A22" s="20" t="s">
+    <row r="21" spans="1:18" s="123" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="121" t="s">
+        <v>195</v>
+      </c>
+      <c r="B21" s="122"/>
+      <c r="C21" s="122"/>
+      <c r="D21" s="122"/>
+      <c r="E21" s="122"/>
+      <c r="F21" s="133"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:18" s="123" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="124" t="s">
+        <v>191</v>
+      </c>
+      <c r="B22" s="125"/>
+      <c r="C22" s="126" t="s">
+        <v>173</v>
+      </c>
+      <c r="D22" s="126"/>
+      <c r="E22" s="126"/>
+      <c r="F22" s="134"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:18" s="123" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="127" t="s">
+        <v>192</v>
+      </c>
+      <c r="B23" s="128"/>
+      <c r="C23" s="129" t="s">
+        <v>198</v>
+      </c>
+      <c r="D23" s="130"/>
+      <c r="E23" s="131"/>
+      <c r="F23" s="132"/>
+    </row>
+    <row r="24" spans="1:18" s="123" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="127" t="s">
+        <v>193</v>
+      </c>
+      <c r="B24" s="128"/>
+      <c r="C24" s="140" t="s">
+        <v>199</v>
+      </c>
+      <c r="D24" s="141"/>
+      <c r="E24" s="142"/>
+      <c r="F24" s="132"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A25" s="6"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A26" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="62"/>
-      <c r="O22" s="62"/>
-      <c r="P22" s="62"/>
-      <c r="Q22" s="41"/>
-      <c r="R22" s="41"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A23" s="113" t="s">
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="40"/>
+      <c r="N26" s="62"/>
+      <c r="O26" s="62"/>
+      <c r="P26" s="62"/>
+      <c r="Q26" s="41"/>
+      <c r="R26" s="41"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A27" s="112" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="113" t="s">
+      <c r="B27" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="115" t="s">
+      <c r="C27" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="113" t="s">
+      <c r="D27" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="118" t="s">
+      <c r="E27" s="115" t="s">
         <v>174</v>
       </c>
-      <c r="F23" s="113" t="s">
+      <c r="F27" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="113" t="s">
+      <c r="G27" s="112" t="s">
         <v>117</v>
       </c>
-      <c r="H23" s="116" t="s">
+      <c r="H27" s="110" t="s">
         <v>78</v>
       </c>
-      <c r="I23" s="117"/>
-      <c r="J23" s="116" t="s">
+      <c r="I27" s="111"/>
+      <c r="J27" s="110" t="s">
         <v>17</v>
       </c>
-      <c r="K23" s="117"/>
-      <c r="L23" s="36" t="s">
+      <c r="K27" s="111"/>
+      <c r="L27" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="M23" s="113" t="s">
+      <c r="M27" s="112" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A24" s="114"/>
-      <c r="B24" s="114"/>
-      <c r="C24" s="114"/>
-      <c r="D24" s="114"/>
-      <c r="E24" s="119"/>
-      <c r="F24" s="114"/>
-      <c r="G24" s="114"/>
-      <c r="H24" s="31" t="s">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A28" s="113"/>
+      <c r="B28" s="113"/>
+      <c r="C28" s="113"/>
+      <c r="D28" s="113"/>
+      <c r="E28" s="116"/>
+      <c r="F28" s="113"/>
+      <c r="G28" s="113"/>
+      <c r="H28" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="I24" s="31" t="s">
+      <c r="I28" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="J24" s="31" t="s">
+      <c r="J28" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="K24" s="31" t="s">
+      <c r="K28" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="L24" s="31" t="s">
+      <c r="L28" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="M24" s="114"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A25" s="7">
+      <c r="M28" s="113"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A29" s="7">
         <v>1</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B29" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D29" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="E25" s="25"/>
-      <c r="F25" s="92" t="s">
+      <c r="E29" s="25"/>
+      <c r="F29" s="91" t="s">
         <v>140</v>
       </c>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25">
+      <c r="G29" s="25"/>
+      <c r="H29" s="25">
         <v>0</v>
       </c>
-      <c r="I25" s="32">
+      <c r="I29" s="32">
         <v>10</v>
       </c>
-      <c r="J25" s="25"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="9"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A26" s="10">
-        <f t="shared" ref="A26:A31" si="0">A25+1</f>
+      <c r="J29" s="25"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="9"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A30" s="10">
+        <f t="shared" ref="A30:A32" si="0">A29+1</f>
         <v>2</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B30" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C30" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D30" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="E26" s="26"/>
-      <c r="F26" s="93"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="22">
+      <c r="E30" s="26"/>
+      <c r="F30" s="92"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="22">
         <v>0</v>
       </c>
-      <c r="K26" s="33">
+      <c r="K30" s="33">
         <v>100</v>
       </c>
-      <c r="L26" s="33"/>
-      <c r="M26" s="12"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A27" s="10">
+      <c r="L30" s="33"/>
+      <c r="M30" s="12"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A31" s="10">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B31" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="27" t="s">
+      <c r="C31" s="13"/>
+      <c r="D31" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="E27" s="27"/>
-      <c r="F27" s="94"/>
-      <c r="G27" s="27" t="b">
+      <c r="E31" s="27"/>
+      <c r="F31" s="93"/>
+      <c r="G31" s="27" t="b">
         <v>1</v>
       </c>
-      <c r="H27" s="22"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="14"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A28" s="10">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B28" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="E28" s="89"/>
-      <c r="F28" s="95"/>
-      <c r="G28" s="89"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="14"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A29" s="10"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="94"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="34"/>
-      <c r="M29" s="14"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A30" s="10"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="94"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="14"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A31" s="10"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="94"/>
-      <c r="G31" s="27"/>
       <c r="H31" s="22"/>
       <c r="I31" s="33"/>
       <c r="J31" s="22"/>
@@ -4238,13 +4566,20 @@
       <c r="M31" s="14"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A32" s="10"/>
-      <c r="B32" s="23"/>
+      <c r="A32" s="10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>104</v>
+      </c>
       <c r="C32" s="13"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
+      <c r="D32" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E32" s="89"/>
       <c r="F32" s="94"/>
-      <c r="G32" s="27"/>
+      <c r="G32" s="89"/>
       <c r="H32" s="22"/>
       <c r="I32" s="33"/>
       <c r="J32" s="22"/>
@@ -4258,7 +4593,7 @@
       <c r="C33" s="13"/>
       <c r="D33" s="27"/>
       <c r="E33" s="27"/>
-      <c r="F33" s="94"/>
+      <c r="F33" s="93"/>
       <c r="G33" s="27"/>
       <c r="H33" s="26"/>
       <c r="I33" s="34"/>
@@ -4273,7 +4608,7 @@
       <c r="C34" s="13"/>
       <c r="D34" s="27"/>
       <c r="E34" s="27"/>
-      <c r="F34" s="94"/>
+      <c r="F34" s="93"/>
       <c r="G34" s="27"/>
       <c r="H34" s="22"/>
       <c r="I34" s="33"/>
@@ -4288,7 +4623,7 @@
       <c r="C35" s="13"/>
       <c r="D35" s="27"/>
       <c r="E35" s="27"/>
-      <c r="F35" s="94"/>
+      <c r="F35" s="93"/>
       <c r="G35" s="27"/>
       <c r="H35" s="22"/>
       <c r="I35" s="33"/>
@@ -4303,7 +4638,7 @@
       <c r="C36" s="13"/>
       <c r="D36" s="27"/>
       <c r="E36" s="27"/>
-      <c r="F36" s="94"/>
+      <c r="F36" s="93"/>
       <c r="G36" s="27"/>
       <c r="H36" s="22"/>
       <c r="I36" s="33"/>
@@ -4318,13 +4653,13 @@
       <c r="C37" s="13"/>
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
-      <c r="F37" s="94"/>
+      <c r="F37" s="93"/>
       <c r="G37" s="27"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="33"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="33"/>
-      <c r="L37" s="33"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="34"/>
+      <c r="L37" s="34"/>
       <c r="M37" s="14"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.15">
@@ -4333,7 +4668,7 @@
       <c r="C38" s="13"/>
       <c r="D38" s="27"/>
       <c r="E38" s="27"/>
-      <c r="F38" s="94"/>
+      <c r="F38" s="93"/>
       <c r="G38" s="27"/>
       <c r="H38" s="22"/>
       <c r="I38" s="33"/>
@@ -4348,13 +4683,13 @@
       <c r="C39" s="13"/>
       <c r="D39" s="27"/>
       <c r="E39" s="27"/>
-      <c r="F39" s="94"/>
+      <c r="F39" s="93"/>
       <c r="G39" s="27"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="26"/>
-      <c r="K39" s="34"/>
-      <c r="L39" s="34"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="33"/>
       <c r="M39" s="14"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.15">
@@ -4363,7 +4698,7 @@
       <c r="C40" s="13"/>
       <c r="D40" s="27"/>
       <c r="E40" s="27"/>
-      <c r="F40" s="94"/>
+      <c r="F40" s="93"/>
       <c r="G40" s="27"/>
       <c r="H40" s="22"/>
       <c r="I40" s="33"/>
@@ -4378,7 +4713,7 @@
       <c r="C41" s="13"/>
       <c r="D41" s="27"/>
       <c r="E41" s="27"/>
-      <c r="F41" s="94"/>
+      <c r="F41" s="93"/>
       <c r="G41" s="27"/>
       <c r="H41" s="22"/>
       <c r="I41" s="33"/>
@@ -4393,7 +4728,7 @@
       <c r="C42" s="13"/>
       <c r="D42" s="27"/>
       <c r="E42" s="27"/>
-      <c r="F42" s="94"/>
+      <c r="F42" s="93"/>
       <c r="G42" s="27"/>
       <c r="H42" s="22"/>
       <c r="I42" s="33"/>
@@ -4408,13 +4743,13 @@
       <c r="C43" s="13"/>
       <c r="D43" s="27"/>
       <c r="E43" s="27"/>
-      <c r="F43" s="94"/>
+      <c r="F43" s="93"/>
       <c r="G43" s="27"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="33"/>
-      <c r="L43" s="33"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="34"/>
+      <c r="L43" s="34"/>
       <c r="M43" s="14"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.15">
@@ -4423,13 +4758,13 @@
       <c r="C44" s="13"/>
       <c r="D44" s="27"/>
       <c r="E44" s="27"/>
-      <c r="F44" s="94"/>
+      <c r="F44" s="93"/>
       <c r="G44" s="27"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="26"/>
-      <c r="K44" s="34"/>
-      <c r="L44" s="34"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="33"/>
+      <c r="L44" s="33"/>
       <c r="M44" s="14"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.15">
@@ -4438,7 +4773,7 @@
       <c r="C45" s="13"/>
       <c r="D45" s="27"/>
       <c r="E45" s="27"/>
-      <c r="F45" s="94"/>
+      <c r="F45" s="93"/>
       <c r="G45" s="27"/>
       <c r="H45" s="22"/>
       <c r="I45" s="33"/>
@@ -4453,7 +4788,7 @@
       <c r="C46" s="13"/>
       <c r="D46" s="27"/>
       <c r="E46" s="27"/>
-      <c r="F46" s="94"/>
+      <c r="F46" s="93"/>
       <c r="G46" s="27"/>
       <c r="H46" s="22"/>
       <c r="I46" s="33"/>
@@ -4468,42 +4803,102 @@
       <c r="C47" s="13"/>
       <c r="D47" s="27"/>
       <c r="E47" s="27"/>
-      <c r="F47" s="94"/>
+      <c r="F47" s="93"/>
       <c r="G47" s="27"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="26"/>
-      <c r="K47" s="34"/>
-      <c r="L47" s="34"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="33"/>
+      <c r="L47" s="33"/>
       <c r="M47" s="14"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A48" s="15"/>
-      <c r="B48" s="24"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="28"/>
-      <c r="F48" s="96"/>
-      <c r="G48" s="28"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="35"/>
-      <c r="J48" s="24"/>
-      <c r="K48" s="35"/>
-      <c r="L48" s="35"/>
-      <c r="M48" s="17"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="93"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="34"/>
+      <c r="J48" s="26"/>
+      <c r="K48" s="34"/>
+      <c r="L48" s="34"/>
+      <c r="M48" s="14"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A49" s="10"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="93"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="33"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="33"/>
+      <c r="L49" s="33"/>
+      <c r="M49" s="14"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A50" s="10"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="93"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="33"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="33"/>
+      <c r="L50" s="33"/>
+      <c r="M50" s="14"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A51" s="10"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="93"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="34"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="34"/>
+      <c r="L51" s="34"/>
+      <c r="M51" s="14"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A52" s="15"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="95"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="24"/>
+      <c r="K52" s="35"/>
+      <c r="L52" s="35"/>
+      <c r="M52" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="M23:M24"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="E27:E28"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -4539,7 +4934,7 @@
           <x14:formula1>
             <xm:f>config!$C$5:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F25:F48</xm:sqref>
+          <xm:sqref>F29:F52</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4552,10 +4947,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4587,7 +4982,7 @@
     <col min="26" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.15">
       <c r="A1" s="18" t="s">
         <v>30</v>
       </c>
@@ -4595,17 +4990,17 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -4615,7 +5010,7 @@
       <c r="E5" s="61"/>
       <c r="G5" s="29"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -4627,7 +5022,7 @@
       <c r="E6" s="61"/>
       <c r="G6" s="29"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>88</v>
       </c>
@@ -4643,7 +5038,7 @@
       <c r="J7" s="61"/>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -4655,7 +5050,7 @@
       <c r="E8" s="61"/>
       <c r="G8" s="29"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>155</v>
       </c>
@@ -4663,23 +5058,23 @@
       <c r="C9" s="90" t="s">
         <v>164</v>
       </c>
-      <c r="D9" s="104"/>
+      <c r="D9" s="103"/>
       <c r="E9" s="61"/>
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="63" t="s">
         <v>142</v>
       </c>
       <c r="B10" s="65"/>
-      <c r="C10" s="102" t="s">
+      <c r="C10" s="101" t="s">
         <v>173</v>
       </c>
-      <c r="D10" s="103"/>
+      <c r="D10" s="102"/>
       <c r="E10" s="61"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
@@ -4688,7 +5083,7 @@
       <c r="D11" s="37"/>
       <c r="E11" s="61"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
         <v>106</v>
       </c>
@@ -4699,235 +5094,229 @@
       <c r="D12" s="37"/>
       <c r="E12" s="61"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="6"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A14" s="6"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A15" s="63" t="s">
+    <row r="14" spans="1:11" s="123" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="121" t="s">
+        <v>195</v>
+      </c>
+      <c r="B14" s="122"/>
+      <c r="C14" s="122"/>
+      <c r="D14" s="122"/>
+      <c r="E14" s="122"/>
+      <c r="F14" s="133"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" s="123" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="124" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15" s="125"/>
+      <c r="C15" s="126" t="s">
+        <v>173</v>
+      </c>
+      <c r="D15" s="126"/>
+      <c r="E15" s="126"/>
+      <c r="F15" s="134"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" s="123" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="127" t="s">
+        <v>192</v>
+      </c>
+      <c r="B16" s="128"/>
+      <c r="C16" s="129" t="s">
+        <v>198</v>
+      </c>
+      <c r="D16" s="130"/>
+      <c r="E16" s="131"/>
+      <c r="F16" s="132"/>
+    </row>
+    <row r="17" spans="1:13" s="123" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="127" t="s">
+        <v>193</v>
+      </c>
+      <c r="B17" s="128"/>
+      <c r="C17" s="140" t="s">
+        <v>199</v>
+      </c>
+      <c r="D17" s="141"/>
+      <c r="E17" s="142"/>
+      <c r="F17" s="132"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A18" s="6"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A19" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="B15" s="64"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="65"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A16" s="118" t="s">
+      <c r="B19" s="64"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="64"/>
+      <c r="I19" s="64"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="65"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A20" s="115" t="s">
         <v>119</v>
       </c>
-      <c r="B16" s="118" t="s">
+      <c r="B20" s="115" t="s">
         <v>120</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C20" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="D16" s="118" t="s">
+      <c r="D20" s="115" t="s">
         <v>108</v>
       </c>
-      <c r="E16" s="118" t="s">
+      <c r="E20" s="115" t="s">
         <v>174</v>
       </c>
-      <c r="F16" s="118" t="s">
+      <c r="F20" s="115" t="s">
         <v>139</v>
       </c>
-      <c r="G16" s="118" t="s">
+      <c r="G20" s="115" t="s">
         <v>138</v>
       </c>
-      <c r="H16" s="120" t="s">
+      <c r="H20" s="120" t="s">
         <v>123</v>
       </c>
-      <c r="I16" s="121"/>
-      <c r="J16" s="122" t="s">
+      <c r="I20" s="118"/>
+      <c r="J20" s="117" t="s">
         <v>124</v>
       </c>
-      <c r="K16" s="121"/>
-      <c r="L16" s="66" t="s">
+      <c r="K20" s="118"/>
+      <c r="L20" s="66" t="s">
         <v>125</v>
       </c>
-      <c r="M16" s="118" t="s">
+      <c r="M20" s="115" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A17" s="123"/>
-      <c r="B17" s="123"/>
-      <c r="C17" s="68" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A21" s="119"/>
+      <c r="B21" s="119"/>
+      <c r="C21" s="68" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="123"/>
-      <c r="E17" s="119"/>
-      <c r="F17" s="123"/>
-      <c r="G17" s="123"/>
-      <c r="H17" s="69" t="s">
+      <c r="D21" s="119"/>
+      <c r="E21" s="116"/>
+      <c r="F21" s="119"/>
+      <c r="G21" s="119"/>
+      <c r="H21" s="69" t="s">
         <v>127</v>
       </c>
-      <c r="I17" s="69" t="s">
+      <c r="I21" s="69" t="s">
         <v>128</v>
       </c>
-      <c r="J17" s="69" t="s">
+      <c r="J21" s="69" t="s">
         <v>129</v>
       </c>
-      <c r="K17" s="69" t="s">
+      <c r="K21" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="L17" s="70" t="s">
+      <c r="L21" s="70" t="s">
         <v>131</v>
       </c>
-      <c r="M17" s="123"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A18" s="71">
+      <c r="M21" s="119"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A22" s="71">
         <v>1</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B22" s="72" t="s">
         <v>134</v>
       </c>
-      <c r="C18" s="73" t="s">
+      <c r="C22" s="73" t="s">
         <v>132</v>
       </c>
-      <c r="D18" s="74" t="s">
+      <c r="D22" s="74" t="s">
         <v>109</v>
       </c>
-      <c r="E18" s="74"/>
-      <c r="F18" s="97" t="s">
+      <c r="E22" s="74"/>
+      <c r="F22" s="96" t="s">
         <v>140</v>
       </c>
-      <c r="G18" s="74"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="74"/>
-      <c r="J18" s="74"/>
-      <c r="K18" s="74"/>
-      <c r="L18" s="74"/>
-      <c r="M18" s="75"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A19" s="71">
-        <v>2</v>
-      </c>
-      <c r="B19" s="72" t="s">
-        <v>135</v>
-      </c>
-      <c r="C19" s="73" t="s">
-        <v>133</v>
-      </c>
-      <c r="D19" s="74" t="s">
-        <v>111</v>
-      </c>
-      <c r="E19" s="74"/>
-      <c r="F19" s="97"/>
-      <c r="G19" s="74"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="72"/>
-      <c r="J19" s="72"/>
-      <c r="K19" s="72"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="75"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A20" s="71">
-        <v>3</v>
-      </c>
-      <c r="B20" s="76" t="s">
-        <v>136</v>
-      </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="77" t="s">
-        <v>113</v>
-      </c>
-      <c r="E20" s="77"/>
-      <c r="F20" s="98"/>
-      <c r="G20" s="77"/>
-      <c r="H20" s="72"/>
-      <c r="I20" s="72"/>
-      <c r="J20" s="72"/>
-      <c r="K20" s="72"/>
-      <c r="L20" s="72"/>
-      <c r="M20" s="78"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A21" s="71">
-        <v>4</v>
-      </c>
-      <c r="B21" s="79" t="s">
-        <v>137</v>
-      </c>
-      <c r="C21" s="80"/>
-      <c r="D21" s="81" t="s">
-        <v>115</v>
-      </c>
-      <c r="E21" s="81"/>
-      <c r="F21" s="101"/>
-      <c r="G21" s="81"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="72"/>
-      <c r="L21" s="72"/>
-      <c r="M21" s="82"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A22" s="71"/>
-      <c r="B22" s="79"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="81"/>
-      <c r="E22" s="81"/>
-      <c r="F22" s="99"/>
-      <c r="G22" s="81"/>
+      <c r="G22" s="74"/>
       <c r="H22" s="74"/>
       <c r="I22" s="74"/>
       <c r="J22" s="74"/>
       <c r="K22" s="74"/>
       <c r="L22" s="74"/>
-      <c r="M22" s="82"/>
+      <c r="M22" s="75"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A23" s="71"/>
-      <c r="B23" s="79"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="81"/>
-      <c r="E23" s="81"/>
-      <c r="F23" s="99"/>
-      <c r="G23" s="81"/>
+      <c r="A23" s="71">
+        <v>2</v>
+      </c>
+      <c r="B23" s="72" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="D23" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="74"/>
+      <c r="F23" s="96"/>
+      <c r="G23" s="74"/>
       <c r="H23" s="72"/>
       <c r="I23" s="72"/>
       <c r="J23" s="72"/>
       <c r="K23" s="72"/>
       <c r="L23" s="72"/>
-      <c r="M23" s="82"/>
+      <c r="M23" s="75"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A24" s="71"/>
-      <c r="B24" s="79"/>
-      <c r="C24" s="80"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="99"/>
-      <c r="G24" s="81"/>
+      <c r="A24" s="71">
+        <v>3</v>
+      </c>
+      <c r="B24" s="76" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" s="54"/>
+      <c r="D24" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="E24" s="77"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="77"/>
       <c r="H24" s="72"/>
       <c r="I24" s="72"/>
       <c r="J24" s="72"/>
       <c r="K24" s="72"/>
       <c r="L24" s="72"/>
-      <c r="M24" s="82"/>
+      <c r="M24" s="78"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A25" s="71"/>
-      <c r="B25" s="79"/>
+      <c r="A25" s="71">
+        <v>4</v>
+      </c>
+      <c r="B25" s="79" t="s">
+        <v>137</v>
+      </c>
       <c r="C25" s="80"/>
-      <c r="D25" s="81"/>
+      <c r="D25" s="81" t="s">
+        <v>115</v>
+      </c>
       <c r="E25" s="81"/>
-      <c r="F25" s="99"/>
+      <c r="F25" s="100"/>
       <c r="G25" s="81"/>
       <c r="H25" s="72"/>
       <c r="I25" s="72"/>
@@ -4942,7 +5331,7 @@
       <c r="C26" s="80"/>
       <c r="D26" s="81"/>
       <c r="E26" s="81"/>
-      <c r="F26" s="99"/>
+      <c r="F26" s="98"/>
       <c r="G26" s="81"/>
       <c r="H26" s="74"/>
       <c r="I26" s="74"/>
@@ -4957,7 +5346,7 @@
       <c r="C27" s="80"/>
       <c r="D27" s="81"/>
       <c r="E27" s="81"/>
-      <c r="F27" s="99"/>
+      <c r="F27" s="98"/>
       <c r="G27" s="81"/>
       <c r="H27" s="72"/>
       <c r="I27" s="72"/>
@@ -4972,7 +5361,7 @@
       <c r="C28" s="80"/>
       <c r="D28" s="81"/>
       <c r="E28" s="81"/>
-      <c r="F28" s="99"/>
+      <c r="F28" s="98"/>
       <c r="G28" s="81"/>
       <c r="H28" s="72"/>
       <c r="I28" s="72"/>
@@ -4987,7 +5376,7 @@
       <c r="C29" s="80"/>
       <c r="D29" s="81"/>
       <c r="E29" s="81"/>
-      <c r="F29" s="99"/>
+      <c r="F29" s="98"/>
       <c r="G29" s="81"/>
       <c r="H29" s="72"/>
       <c r="I29" s="72"/>
@@ -5002,13 +5391,13 @@
       <c r="C30" s="80"/>
       <c r="D30" s="81"/>
       <c r="E30" s="81"/>
-      <c r="F30" s="99"/>
+      <c r="F30" s="98"/>
       <c r="G30" s="81"/>
-      <c r="H30" s="72"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="72"/>
-      <c r="K30" s="72"/>
-      <c r="L30" s="72"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="74"/>
+      <c r="K30" s="74"/>
+      <c r="L30" s="74"/>
       <c r="M30" s="82"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.15">
@@ -5017,7 +5406,7 @@
       <c r="C31" s="80"/>
       <c r="D31" s="81"/>
       <c r="E31" s="81"/>
-      <c r="F31" s="99"/>
+      <c r="F31" s="98"/>
       <c r="G31" s="81"/>
       <c r="H31" s="72"/>
       <c r="I31" s="72"/>
@@ -5032,13 +5421,13 @@
       <c r="C32" s="80"/>
       <c r="D32" s="81"/>
       <c r="E32" s="81"/>
-      <c r="F32" s="99"/>
+      <c r="F32" s="98"/>
       <c r="G32" s="81"/>
-      <c r="H32" s="74"/>
-      <c r="I32" s="74"/>
-      <c r="J32" s="74"/>
-      <c r="K32" s="74"/>
-      <c r="L32" s="74"/>
+      <c r="H32" s="72"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="72"/>
+      <c r="K32" s="72"/>
+      <c r="L32" s="72"/>
       <c r="M32" s="82"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.15">
@@ -5047,7 +5436,7 @@
       <c r="C33" s="80"/>
       <c r="D33" s="81"/>
       <c r="E33" s="81"/>
-      <c r="F33" s="99"/>
+      <c r="F33" s="98"/>
       <c r="G33" s="81"/>
       <c r="H33" s="72"/>
       <c r="I33" s="72"/>
@@ -5062,7 +5451,7 @@
       <c r="C34" s="80"/>
       <c r="D34" s="81"/>
       <c r="E34" s="81"/>
-      <c r="F34" s="99"/>
+      <c r="F34" s="98"/>
       <c r="G34" s="81"/>
       <c r="H34" s="72"/>
       <c r="I34" s="72"/>
@@ -5077,7 +5466,7 @@
       <c r="C35" s="80"/>
       <c r="D35" s="81"/>
       <c r="E35" s="81"/>
-      <c r="F35" s="99"/>
+      <c r="F35" s="98"/>
       <c r="G35" s="81"/>
       <c r="H35" s="72"/>
       <c r="I35" s="72"/>
@@ -5092,13 +5481,13 @@
       <c r="C36" s="80"/>
       <c r="D36" s="81"/>
       <c r="E36" s="81"/>
-      <c r="F36" s="99"/>
+      <c r="F36" s="98"/>
       <c r="G36" s="81"/>
-      <c r="H36" s="72"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="72"/>
-      <c r="K36" s="72"/>
-      <c r="L36" s="72"/>
+      <c r="H36" s="74"/>
+      <c r="I36" s="74"/>
+      <c r="J36" s="74"/>
+      <c r="K36" s="74"/>
+      <c r="L36" s="74"/>
       <c r="M36" s="82"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.15">
@@ -5107,13 +5496,13 @@
       <c r="C37" s="80"/>
       <c r="D37" s="81"/>
       <c r="E37" s="81"/>
-      <c r="F37" s="99"/>
+      <c r="F37" s="98"/>
       <c r="G37" s="81"/>
-      <c r="H37" s="74"/>
-      <c r="I37" s="74"/>
-      <c r="J37" s="74"/>
-      <c r="K37" s="74"/>
-      <c r="L37" s="74"/>
+      <c r="H37" s="72"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="72"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="72"/>
       <c r="M37" s="82"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.15">
@@ -5122,7 +5511,7 @@
       <c r="C38" s="80"/>
       <c r="D38" s="81"/>
       <c r="E38" s="81"/>
-      <c r="F38" s="99"/>
+      <c r="F38" s="98"/>
       <c r="G38" s="81"/>
       <c r="H38" s="72"/>
       <c r="I38" s="72"/>
@@ -5137,7 +5526,7 @@
       <c r="C39" s="80"/>
       <c r="D39" s="81"/>
       <c r="E39" s="81"/>
-      <c r="F39" s="99"/>
+      <c r="F39" s="98"/>
       <c r="G39" s="81"/>
       <c r="H39" s="72"/>
       <c r="I39" s="72"/>
@@ -5152,41 +5541,101 @@
       <c r="C40" s="80"/>
       <c r="D40" s="81"/>
       <c r="E40" s="81"/>
-      <c r="F40" s="99"/>
+      <c r="F40" s="98"/>
       <c r="G40" s="81"/>
-      <c r="H40" s="74"/>
-      <c r="I40" s="74"/>
-      <c r="J40" s="74"/>
-      <c r="K40" s="74"/>
-      <c r="L40" s="74"/>
+      <c r="H40" s="72"/>
+      <c r="I40" s="72"/>
+      <c r="J40" s="72"/>
+      <c r="K40" s="72"/>
+      <c r="L40" s="72"/>
       <c r="M40" s="82"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A41" s="83"/>
-      <c r="B41" s="84"/>
-      <c r="C41" s="85"/>
-      <c r="D41" s="86"/>
-      <c r="E41" s="86"/>
-      <c r="F41" s="100"/>
-      <c r="G41" s="86"/>
-      <c r="H41" s="87"/>
-      <c r="I41" s="87"/>
-      <c r="J41" s="87"/>
-      <c r="K41" s="87"/>
-      <c r="L41" s="87"/>
-      <c r="M41" s="88"/>
+      <c r="A41" s="71"/>
+      <c r="B41" s="79"/>
+      <c r="C41" s="80"/>
+      <c r="D41" s="81"/>
+      <c r="E41" s="81"/>
+      <c r="F41" s="98"/>
+      <c r="G41" s="81"/>
+      <c r="H41" s="74"/>
+      <c r="I41" s="74"/>
+      <c r="J41" s="74"/>
+      <c r="K41" s="74"/>
+      <c r="L41" s="74"/>
+      <c r="M41" s="82"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A42" s="71"/>
+      <c r="B42" s="79"/>
+      <c r="C42" s="80"/>
+      <c r="D42" s="81"/>
+      <c r="E42" s="81"/>
+      <c r="F42" s="98"/>
+      <c r="G42" s="81"/>
+      <c r="H42" s="72"/>
+      <c r="I42" s="72"/>
+      <c r="J42" s="72"/>
+      <c r="K42" s="72"/>
+      <c r="L42" s="72"/>
+      <c r="M42" s="82"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A43" s="71"/>
+      <c r="B43" s="79"/>
+      <c r="C43" s="80"/>
+      <c r="D43" s="81"/>
+      <c r="E43" s="81"/>
+      <c r="F43" s="98"/>
+      <c r="G43" s="81"/>
+      <c r="H43" s="72"/>
+      <c r="I43" s="72"/>
+      <c r="J43" s="72"/>
+      <c r="K43" s="72"/>
+      <c r="L43" s="72"/>
+      <c r="M43" s="82"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A44" s="71"/>
+      <c r="B44" s="79"/>
+      <c r="C44" s="80"/>
+      <c r="D44" s="81"/>
+      <c r="E44" s="81"/>
+      <c r="F44" s="98"/>
+      <c r="G44" s="81"/>
+      <c r="H44" s="74"/>
+      <c r="I44" s="74"/>
+      <c r="J44" s="74"/>
+      <c r="K44" s="74"/>
+      <c r="L44" s="74"/>
+      <c r="M44" s="82"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A45" s="83"/>
+      <c r="B45" s="84"/>
+      <c r="C45" s="85"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="99"/>
+      <c r="G45" s="86"/>
+      <c r="H45" s="87"/>
+      <c r="I45" s="87"/>
+      <c r="J45" s="87"/>
+      <c r="K45" s="87"/>
+      <c r="L45" s="87"/>
+      <c r="M45" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="E20:E21"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -5213,7 +5662,7 @@
           <x14:formula1>
             <xm:f>config!$C$5:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F18:F41</xm:sqref>
+          <xm:sqref>F22:F45</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>